<commit_message>
- generated results by varying dictionary size (K) in KSVD algorithm to study the variation in compression and avg. sparsity with varying K
</commit_message>
<xml_diff>
--- a/output/to_publish/table3.xlsx
+++ b/output/to_publish/table3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="iono" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="43">
   <si>
     <t>Dataset</t>
   </si>
@@ -128,6 +128,30 @@
   </si>
   <si>
     <t>*dl-max algorithm doesn't terminate for this dataset</t>
+  </si>
+  <si>
+    <t>dp-max</t>
+  </si>
+  <si>
+    <t>dl-max</t>
+  </si>
+  <si>
+    <t>dch-max</t>
+  </si>
+  <si>
+    <t>dchperceptron-max</t>
+  </si>
+  <si>
+    <t>dp-mean</t>
+  </si>
+  <si>
+    <t>dl-mean</t>
+  </si>
+  <si>
+    <t>dch-mean</t>
+  </si>
+  <si>
+    <t>dchperceptron-mean</t>
   </si>
 </sst>
 </file>
@@ -691,6 +715,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -700,10 +728,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1084,11 +1108,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1104,7 +1128,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>0.47460999999999998</v>
@@ -1116,7 +1140,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>0.39995000000000003</v>
@@ -1128,7 +1152,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3">
         <v>0.33937</v>
@@ -1140,7 +1164,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
         <v>0.36843999999999999</v>
@@ -1152,7 +1176,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>0.38612000000000002</v>
@@ -1164,7 +1188,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>0.27786</v>
@@ -1175,7 +1199,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>0.28281000000000001</v>
@@ -1186,7 +1210,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>0.44218000000000002</v>
@@ -1675,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1698,11 +1722,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -1718,7 +1742,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>0.68239000000000005</v>
@@ -1730,7 +1754,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>0.39605000000000001</v>
@@ -1742,7 +1766,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3">
         <v>0.43973000000000001</v>
@@ -1754,7 +1778,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
         <v>0.46507999999999999</v>
@@ -1766,7 +1790,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>0.48036000000000001</v>
@@ -1778,7 +1802,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>0.25896999999999998</v>
@@ -1789,7 +1813,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>1.27416</v>
@@ -1800,7 +1824,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>1.2753699999999999</v>
@@ -2245,7 +2269,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2267,11 +2291,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2287,7 +2311,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>0.59226999999999996</v>
@@ -2299,7 +2323,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>0.26766000000000001</v>
@@ -2311,7 +2335,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3">
         <v>0.24956</v>
@@ -2323,7 +2347,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
         <v>0.25840999999999997</v>
@@ -2335,7 +2359,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>0.41049000000000002</v>
@@ -2347,7 +2371,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>0.16011</v>
@@ -2358,7 +2382,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>0.51756999999999997</v>
@@ -2369,7 +2393,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>0.77405000000000002</v>
@@ -2814,7 +2838,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A3" sqref="A3:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2836,11 +2860,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -2856,7 +2880,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>0.72335000000000005</v>
@@ -2868,7 +2892,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3">
         <v>0.41027000000000002</v>
@@ -2880,7 +2904,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3">
         <v>0.19139999999999999</v>
@@ -2892,7 +2916,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
         <v>0.19599</v>
@@ -2904,7 +2928,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>0.47366999999999998</v>
@@ -2916,7 +2940,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>0.21401999999999999</v>
@@ -2927,7 +2951,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>8.1890000000000004E-2</v>
@@ -2938,7 +2962,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>8.6860000000000007E-2</v>
@@ -3382,8 +3406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3405,11 +3429,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -3425,7 +3449,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3">
         <v>0.65900999999999998</v>
@@ -3437,7 +3461,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>26</v>
@@ -3447,7 +3471,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3">
         <v>0.39399000000000001</v>
@@ -3459,7 +3483,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B6" s="3">
         <v>0.38390999999999997</v>
@@ -3471,7 +3495,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3">
         <v>0.44988</v>
@@ -3483,7 +3507,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B8" s="3">
         <v>0.26089000000000001</v>
@@ -3494,7 +3518,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3">
         <v>0.12038</v>
@@ -3505,7 +3529,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3">
         <v>0.13139999999999999</v>
@@ -3526,12 +3550,12 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- used a package to deskew mnist data and store it separately
</commit_message>
<xml_diff>
--- a/output/to_publish/table3.xlsx
+++ b/output/to_publish/table3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="iono" sheetId="1" r:id="rId1"/>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1699,7 +1699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2269,7 +2269,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2838,7 +2838,7 @@
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3406,7 +3406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>